<commit_message>
Add HTML template for displaying wrestlers by number of times picked with sorting and filtering functionality
</commit_message>
<xml_diff>
--- a/wrestlers.xlsx
+++ b/wrestlers.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10311"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10209"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jholenda/PycharmProjects/MarchMatness/GAME/2024/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jholenda/Code/wrestling-management/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5E4194C1-4C9F-AE47-BCA1-DA18A5B55913}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ACBCBE5F-0685-3A46-BA21-B41191629625}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="64000" yWindow="500" windowWidth="25600" windowHeight="21100" xr2:uid="{7FA0CBB2-F3DC-AE4D-9F27-C36B83A9EF09}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="33600" windowHeight="21000" xr2:uid="{7FA0CBB2-F3DC-AE4D-9F27-C36B83A9EF09}"/>
   </bookViews>
   <sheets>
     <sheet name="ALL Wrestlers" sheetId="2" r:id="rId1"/>
@@ -54,7 +54,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="664" uniqueCount="335">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="664" uniqueCount="339">
   <si>
     <t>9-10 Seeds</t>
   </si>
@@ -1059,6 +1059,18 @@
   </si>
   <si>
     <t>(33) Greer, Jordan</t>
+  </si>
+  <si>
+    <t>(1) OToole, Keegan</t>
+  </si>
+  <si>
+    <t>(14) DEmilio, Dylan</t>
+  </si>
+  <si>
+    <t>(29) Anderson, JhaQuan</t>
+  </si>
+  <si>
+    <t>(32) DAlesio, Anthony</t>
   </si>
 </sst>
 </file>
@@ -1423,7 +1435,7 @@
   <dimension ref="A1:J34"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E16" sqref="E16:E17"/>
+      <selection activeCell="H33" sqref="H33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1489,7 +1501,7 @@
         <v>137</v>
       </c>
       <c r="F2" t="s">
-        <v>170</v>
+        <v>335</v>
       </c>
       <c r="G2" t="s">
         <v>203</v>
@@ -1899,7 +1911,7 @@
         <v>84</v>
       </c>
       <c r="D15" t="s">
-        <v>117</v>
+        <v>336</v>
       </c>
       <c r="E15" t="s">
         <v>150</v>
@@ -2391,7 +2403,7 @@
         <v>231</v>
       </c>
       <c r="H30" t="s">
-        <v>264</v>
+        <v>337</v>
       </c>
       <c r="I30" t="s">
         <v>297</v>
@@ -2487,7 +2499,7 @@
         <v>234</v>
       </c>
       <c r="H33" t="s">
-        <v>267</v>
+        <v>338</v>
       </c>
       <c r="I33" t="s">
         <v>300</v>

</xml_diff>